<commit_message>
bugfix: add class structure in control.py. Also did some tests on converting the excel to rule files
</commit_message>
<xml_diff>
--- a/temp/metrics_excel.xlsx
+++ b/temp/metrics_excel.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="550">
   <si>
     <t xml:space="preserve">Enabled</t>
   </si>
@@ -292,6 +292,27 @@
   </si>
   <si>
     <t xml:space="preserve">A Prometheus job has disappeared\n  VALUE = {{ $value }}\n  LABELS = {{ $labels }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Process Exporter Alerts</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum(rate(namedprocess_namegroup_cpu_seconds_total{groupname=~".+"}[1m])) by (groupname, instance) * 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HeavyCpuUsage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum(rate(namedprocess_namegroup_cpu_seconds_total{groupname=~".+"}[1m])) by (groupname, instance) * 100 &gt; 99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heavy CPU Process</t>
   </si>
   <si>
     <t xml:space="preserve">N</t>
@@ -1693,7 +1714,7 @@
     <numFmt numFmtId="166" formatCode="General"/>
     <numFmt numFmtId="167" formatCode="0%"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1791,6 +1812,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF2A6099"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1852,7 +1880,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1883,6 +1911,13 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -1952,7 +1987,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2093,39 +2128,59 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2191,7 +2246,7 @@
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFF4B183"/>
-      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF2A6099"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF92D050"/>
       <rgbColor rgb="FFFFC000"/>
@@ -2223,9 +2278,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>155520</xdr:colOff>
+      <xdr:colOff>152640</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>49320</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2238,13 +2293,13 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1028160" y="181080"/>
-          <a:ext cx="16604640" cy="5297400"/>
+          <a:off x="1032840" y="180720"/>
+          <a:ext cx="16683120" cy="5294880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln w="0">
+        <a:ln>
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -2260,9 +2315,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>189000</xdr:colOff>
+      <xdr:colOff>186120</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>113400</xdr:rowOff>
+      <xdr:rowOff>110520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2275,13 +2330,13 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1028160" y="5985360"/>
-          <a:ext cx="16638120" cy="5710320"/>
+          <a:off x="1032840" y="5985360"/>
+          <a:ext cx="16716600" cy="5707440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln w="0">
+        <a:ln>
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -2302,9 +2357,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1356120</xdr:colOff>
+      <xdr:colOff>1353240</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>185400</xdr:rowOff>
+      <xdr:rowOff>182520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2318,12 +2373,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="380880" y="2032920"/>
-          <a:ext cx="8474040" cy="3305520"/>
+          <a:ext cx="8470800" cy="3302280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln w="0">
+        <a:ln>
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -2339,9 +2394,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>605880</xdr:colOff>
+      <xdr:colOff>603000</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>50040</xdr:rowOff>
+      <xdr:rowOff>47160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2354,13 +2409,13 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8853480" y="2041560"/>
-          <a:ext cx="8341200" cy="3351960"/>
+          <a:off x="8853120" y="2041560"/>
+          <a:ext cx="8338320" cy="3349080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln w="0">
+        <a:ln>
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -2375,12 +2430,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R44"/>
+  <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2985,7 +3040,7 @@
       <c r="Q12" s="26"/>
       <c r="R12" s="27"/>
     </row>
-    <row r="13" s="16" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" s="16" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
@@ -3021,69 +3076,101 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="2" customFormat="true" ht="139.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
-        <v>80</v>
+        <v>18</v>
       </c>
       <c r="B14" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="22" t="n">
+      <c r="E14" s="37" t="n">
         <v>100</v>
       </c>
-      <c r="F14" s="22" t="n">
+      <c r="F14" s="37" t="n">
         <v>0</v>
       </c>
-      <c r="G14" s="22" t="n">
-        <v>95</v>
-      </c>
-      <c r="H14" s="22" t="n">
-        <v>85</v>
-      </c>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
+      <c r="G14" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="37" t="n">
+        <v>99</v>
+      </c>
+      <c r="I14" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="J14" s="36" t="s">
+        <v>81</v>
+      </c>
       <c r="K14" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="L14" s="24"/>
+      <c r="L14" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="M14" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="N14" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="O14" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="P14" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q14" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="R14" s="27" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B15" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D15" s="20"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
+      <c r="E15" s="22" t="n">
+        <v>100</v>
+      </c>
+      <c r="F15" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="22" t="n">
+        <v>95</v>
+      </c>
+      <c r="H15" s="22" t="n">
+        <v>85</v>
+      </c>
       <c r="I15" s="22"/>
       <c r="J15" s="22"/>
-      <c r="K15" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="L15" s="24" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K15" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="L15" s="24"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B16" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="22"/>
@@ -3092,20 +3179,22 @@
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
-      <c r="K16" s="35" t="s">
+      <c r="K16" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="L16" s="24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="L16" s="24"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="22"/>
@@ -3114,45 +3203,43 @@
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
       <c r="J17" s="22"/>
-      <c r="K17" s="35"/>
+      <c r="K17" s="40" t="s">
+        <v>94</v>
+      </c>
       <c r="L17" s="24"/>
     </row>
-    <row r="18" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B18" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>89</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="D18" s="20"/>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>
       <c r="I18" s="22"/>
       <c r="J18" s="22"/>
-      <c r="K18" s="35" t="s">
-        <v>90</v>
-      </c>
+      <c r="K18" s="40"/>
       <c r="L18" s="24"/>
     </row>
-    <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
@@ -3160,97 +3247,97 @@
       <c r="H19" s="22"/>
       <c r="I19" s="22"/>
       <c r="J19" s="22"/>
-      <c r="K19" s="35" t="s">
-        <v>92</v>
+      <c r="K19" s="40" t="s">
+        <v>97</v>
       </c>
       <c r="L19" s="24"/>
     </row>
-    <row r="20" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="22" t="n">
-        <v>100</v>
-      </c>
-      <c r="F20" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" s="22" t="n">
-        <v>90</v>
-      </c>
-      <c r="H20" s="22" t="n">
-        <v>80</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
       <c r="I20" s="22"/>
       <c r="J20" s="22"/>
-      <c r="K20" s="35" t="s">
-        <v>94</v>
+      <c r="K20" s="40" t="s">
+        <v>99</v>
       </c>
       <c r="L20" s="24"/>
     </row>
-    <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="22" t="n">
+        <v>100</v>
+      </c>
+      <c r="F21" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="22" t="n">
+        <v>90</v>
+      </c>
+      <c r="H21" s="22" t="n">
         <v>80</v>
       </c>
-      <c r="B21" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
       <c r="I21" s="22"/>
       <c r="J21" s="22"/>
-      <c r="K21" s="35"/>
+      <c r="K21" s="40" t="s">
+        <v>101</v>
+      </c>
       <c r="L21" s="24"/>
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B22" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>96</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="D22" s="20"/>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
       <c r="H22" s="22"/>
       <c r="I22" s="22"/>
       <c r="J22" s="22"/>
-      <c r="K22" s="35" t="s">
-        <v>97</v>
-      </c>
+      <c r="K22" s="40"/>
       <c r="L22" s="24"/>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B23" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
@@ -3258,130 +3345,130 @@
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="J23" s="22"/>
-      <c r="K23" s="35" t="s">
-        <v>99</v>
+      <c r="K23" s="40" t="s">
+        <v>104</v>
       </c>
       <c r="L23" s="24"/>
     </row>
-    <row r="24" s="16" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="15"/>
-      <c r="O24" s="17"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="24"/>
+    <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="L24" s="24"/>
+    </row>
+    <row r="25" s="16" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="15"/>
+      <c r="O25" s="17"/>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B26" s="34" t="s">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="B26" s="39" t="s">
+        <v>107</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>102</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="D26" s="20"/>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
       <c r="H26" s="22"/>
       <c r="I26" s="22"/>
       <c r="J26" s="22"/>
-      <c r="K26" s="35" t="s">
-        <v>103</v>
-      </c>
+      <c r="K26" s="40"/>
       <c r="L26" s="24"/>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" s="34" t="s">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="B27" s="39" t="s">
+        <v>107</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D27" s="20"/>
+        <v>108</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>109</v>
+      </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
       <c r="H27" s="22"/>
       <c r="I27" s="22"/>
       <c r="J27" s="22"/>
-      <c r="K27" s="35"/>
+      <c r="K27" s="40" t="s">
+        <v>110</v>
+      </c>
       <c r="L27" s="24"/>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" s="34" t="s">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="B28" s="39" t="s">
+        <v>107</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>105</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="D28" s="20"/>
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
       <c r="H28" s="22"/>
       <c r="I28" s="22"/>
       <c r="J28" s="22"/>
-      <c r="K28" s="35" t="s">
-        <v>106</v>
-      </c>
+      <c r="K28" s="40"/>
       <c r="L28" s="24"/>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29" s="34" t="s">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="B29" s="39" t="s">
+        <v>107</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
@@ -3389,67 +3476,67 @@
       <c r="H29" s="22"/>
       <c r="I29" s="22"/>
       <c r="J29" s="22"/>
-      <c r="K29" s="35" t="s">
-        <v>108</v>
+      <c r="K29" s="40" t="s">
+        <v>113</v>
       </c>
       <c r="L29" s="24"/>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" s="34" t="s">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="B30" s="39" t="s">
+        <v>107</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="D30" s="20"/>
+        <v>111</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>114</v>
+      </c>
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
       <c r="H30" s="22"/>
       <c r="I30" s="22"/>
       <c r="J30" s="22"/>
-      <c r="K30" s="35"/>
+      <c r="K30" s="40" t="s">
+        <v>115</v>
+      </c>
       <c r="L30" s="24"/>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B31" s="34" t="s">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="B31" s="39" t="s">
+        <v>107</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>105</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="D31" s="20"/>
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
       <c r="H31" s="22"/>
       <c r="I31" s="22"/>
       <c r="J31" s="22"/>
-      <c r="K31" s="35" t="s">
-        <v>110</v>
-      </c>
+      <c r="K31" s="40"/>
       <c r="L31" s="24"/>
     </row>
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" s="34" t="s">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="B32" s="39" t="s">
+        <v>107</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
@@ -3457,42 +3544,44 @@
       <c r="H32" s="22"/>
       <c r="I32" s="22"/>
       <c r="J32" s="22"/>
-      <c r="K32" s="35" t="s">
-        <v>111</v>
+      <c r="K32" s="40" t="s">
+        <v>117</v>
       </c>
       <c r="L32" s="24"/>
     </row>
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" s="34" t="s">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="B33" s="39" t="s">
+        <v>107</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="D33" s="20"/>
+        <v>116</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>114</v>
+      </c>
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
       <c r="H33" s="22"/>
       <c r="I33" s="22"/>
       <c r="J33" s="22"/>
-      <c r="K33" s="35" t="s">
-        <v>113</v>
+      <c r="K33" s="40" t="s">
+        <v>118</v>
       </c>
       <c r="L33" s="24"/>
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B34" s="34" t="s">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="B34" s="39" t="s">
+        <v>107</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D34" s="20"/>
       <c r="E34" s="22"/>
@@ -3501,45 +3590,43 @@
       <c r="H34" s="22"/>
       <c r="I34" s="22"/>
       <c r="J34" s="22"/>
-      <c r="K34" s="35"/>
+      <c r="K34" s="40" t="s">
+        <v>120</v>
+      </c>
       <c r="L34" s="24"/>
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B35" s="34" t="s">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="B35" s="39" t="s">
+        <v>107</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>115</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="D35" s="20"/>
       <c r="E35" s="22"/>
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
       <c r="H35" s="22"/>
       <c r="I35" s="22"/>
       <c r="J35" s="22"/>
-      <c r="K35" s="35" t="s">
-        <v>116</v>
-      </c>
+      <c r="K35" s="40"/>
       <c r="L35" s="24"/>
     </row>
     <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B36" s="34" t="s">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="B36" s="39" t="s">
+        <v>107</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
@@ -3547,67 +3634,67 @@
       <c r="H36" s="22"/>
       <c r="I36" s="22"/>
       <c r="J36" s="22"/>
-      <c r="K36" s="35" t="s">
-        <v>118</v>
+      <c r="K36" s="40" t="s">
+        <v>123</v>
       </c>
       <c r="L36" s="24"/>
     </row>
     <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B37" s="34" t="s">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="B37" s="39" t="s">
+        <v>107</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="D37" s="20"/>
+        <v>121</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>124</v>
+      </c>
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
       <c r="H37" s="22"/>
       <c r="I37" s="22"/>
       <c r="J37" s="22"/>
-      <c r="K37" s="35"/>
+      <c r="K37" s="40" t="s">
+        <v>125</v>
+      </c>
       <c r="L37" s="24"/>
     </row>
     <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38" s="34" t="s">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="B38" s="39" t="s">
+        <v>107</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>115</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="D38" s="20"/>
       <c r="E38" s="22"/>
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
       <c r="H38" s="22"/>
       <c r="I38" s="22"/>
       <c r="J38" s="22"/>
-      <c r="K38" s="35" t="s">
-        <v>120</v>
-      </c>
+      <c r="K38" s="40"/>
       <c r="L38" s="24"/>
     </row>
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" s="34" t="s">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="B39" s="39" t="s">
+        <v>107</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="E39" s="22"/>
       <c r="F39" s="22"/>
@@ -3615,85 +3702,89 @@
       <c r="H39" s="22"/>
       <c r="I39" s="22"/>
       <c r="J39" s="22"/>
-      <c r="K39" s="35" t="s">
-        <v>121</v>
+      <c r="K39" s="40" t="s">
+        <v>127</v>
       </c>
       <c r="L39" s="24"/>
     </row>
-    <row r="40" s="16" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="15"/>
-      <c r="O40" s="17"/>
-    </row>
-    <row r="41" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="F41" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" s="22" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H41" s="22" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="I41" s="22"/>
-      <c r="J41" s="22"/>
-      <c r="K41" s="35" t="s">
+    <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="D40" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="L41" s="24"/>
-    </row>
-    <row r="42" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="L40" s="24"/>
+    </row>
+    <row r="41" s="16" customFormat="true" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="15"/>
+      <c r="O41" s="17"/>
+    </row>
+    <row r="42" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="18" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B42" s="20"/>
       <c r="C42" s="20" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="D42" s="20"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="22"/>
+      <c r="E42" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="22" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="H42" s="22" t="n">
+        <v>0.75</v>
+      </c>
       <c r="I42" s="22"/>
       <c r="J42" s="22"/>
-      <c r="K42" s="35" t="s">
-        <v>126</v>
+      <c r="K42" s="40" t="s">
+        <v>131</v>
       </c>
       <c r="L42" s="24"/>
     </row>
     <row r="43" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="18" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B43" s="20"/>
       <c r="C43" s="20" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="22"/>
@@ -3702,18 +3793,18 @@
       <c r="H43" s="22"/>
       <c r="I43" s="22"/>
       <c r="J43" s="22"/>
-      <c r="K43" s="35" t="s">
-        <v>128</v>
+      <c r="K43" s="40" t="s">
+        <v>133</v>
       </c>
       <c r="L43" s="24"/>
     </row>
     <row r="44" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="18" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B44" s="20"/>
       <c r="C44" s="20" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="22"/>
@@ -3722,15 +3813,77 @@
       <c r="H44" s="22"/>
       <c r="I44" s="22"/>
       <c r="J44" s="22"/>
-      <c r="K44" s="35" t="s">
-        <v>130</v>
+      <c r="K44" s="40" t="s">
+        <v>135</v>
       </c>
       <c r="L44" s="24"/>
     </row>
+    <row r="45" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D45" s="20"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="L45" s="24"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0"/>
+      <c r="B46" s="0"/>
+      <c r="C46" s="0"/>
+      <c r="D46" s="0"/>
+      <c r="E46" s="0"/>
+      <c r="F46" s="0"/>
+      <c r="G46" s="0"/>
+      <c r="H46" s="0"/>
+      <c r="I46" s="0"/>
+      <c r="J46" s="0"/>
+      <c r="K46" s="0"/>
+      <c r="L46" s="0"/>
+      <c r="M46" s="0"/>
+      <c r="N46" s="0"/>
+      <c r="O46" s="0"/>
+      <c r="P46" s="0"/>
+      <c r="Q46" s="0"/>
+      <c r="R46" s="0"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0"/>
+      <c r="B47" s="0"/>
+      <c r="C47" s="0"/>
+      <c r="D47" s="0"/>
+      <c r="E47" s="0"/>
+      <c r="F47" s="0"/>
+      <c r="G47" s="0"/>
+      <c r="H47" s="0"/>
+      <c r="I47" s="0"/>
+      <c r="J47" s="0"/>
+      <c r="K47" s="0"/>
+      <c r="L47" s="0"/>
+      <c r="M47" s="0"/>
+      <c r="N47" s="0"/>
+      <c r="O47" s="0"/>
+      <c r="P47" s="0"/>
+      <c r="Q47" s="0"/>
+      <c r="R47" s="0"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3746,15 +3899,15 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.56640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3770,275 +3923,275 @@
   </sheetPr>
   <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="102" zoomScaleNormal="102" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="36" width="119.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="36" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="41" width="119.21"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="41" width="11"/>
   </cols>
   <sheetData>
-    <row r="1" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="s">
-        <v>131</v>
+    <row r="1" s="43" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="42" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39" t="s">
-        <v>132</v>
+      <c r="A2" s="44" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="40" t="s">
-        <v>133</v>
+      <c r="A3" s="45" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="40" t="s">
-        <v>134</v>
+      <c r="A4" s="45" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39" t="s">
-        <v>135</v>
+      <c r="A5" s="44" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="40" t="s">
-        <v>136</v>
+      <c r="A6" s="45" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="40" t="s">
-        <v>137</v>
+      <c r="A7" s="45" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="s">
-        <v>138</v>
+      <c r="A8" s="44" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="40" t="s">
-        <v>139</v>
+      <c r="A9" s="45" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="40" t="s">
-        <v>140</v>
+      <c r="A10" s="45" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="39" t="s">
-        <v>141</v>
+      <c r="A11" s="44" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="40" t="s">
-        <v>142</v>
+      <c r="A12" s="45" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="40" t="s">
-        <v>143</v>
+      <c r="A13" s="45" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="40" t="s">
-        <v>144</v>
+      <c r="A14" s="45" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="39" t="s">
-        <v>145</v>
+      <c r="A15" s="44" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="40" t="s">
-        <v>146</v>
+      <c r="A16" s="45" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="40" t="s">
-        <v>147</v>
+      <c r="A17" s="45" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="40" t="s">
-        <v>148</v>
+      <c r="A18" s="45" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="40" t="s">
-        <v>149</v>
+      <c r="A19" s="45" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="39" t="s">
-        <v>150</v>
+      <c r="A20" s="44" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="40" t="s">
-        <v>151</v>
+      <c r="A21" s="45" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="40" t="s">
-        <v>152</v>
+      <c r="A22" s="45" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="40" t="s">
-        <v>153</v>
+      <c r="A23" s="45" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="40" t="s">
-        <v>154</v>
+      <c r="A24" s="45" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="40" t="s">
-        <v>155</v>
+      <c r="A25" s="45" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="40" t="s">
-        <v>156</v>
+      <c r="A26" s="45" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="40" t="s">
-        <v>157</v>
+      <c r="A27" s="45" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="39" t="s">
-        <v>158</v>
+      <c r="A28" s="44" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="40" t="s">
-        <v>159</v>
+      <c r="A29" s="45" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="40" t="s">
-        <v>160</v>
+      <c r="A30" s="45" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="39" t="s">
-        <v>161</v>
+      <c r="A31" s="44" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="40" t="s">
-        <v>162</v>
+      <c r="A32" s="45" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="40" t="s">
-        <v>163</v>
+      <c r="A33" s="45" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="40" t="s">
-        <v>164</v>
+      <c r="A34" s="45" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="40" t="s">
-        <v>165</v>
+      <c r="A35" s="45" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="39" t="s">
-        <v>166</v>
+      <c r="A36" s="44" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="40" t="s">
-        <v>167</v>
+      <c r="A37" s="45" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="40" t="s">
-        <v>168</v>
+      <c r="A38" s="45" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="40" t="s">
-        <v>169</v>
+      <c r="A39" s="45" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="39" t="s">
-        <v>170</v>
+      <c r="A40" s="44" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="40" t="s">
-        <v>171</v>
+      <c r="A41" s="45" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="40" t="s">
-        <v>172</v>
+      <c r="A42" s="45" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="40" t="s">
-        <v>173</v>
+      <c r="A43" s="45" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="40" t="s">
-        <v>174</v>
+      <c r="A44" s="45" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="40" t="s">
-        <v>175</v>
+      <c r="A45" s="45" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="39" t="s">
-        <v>176</v>
+      <c r="A46" s="44" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="40" t="s">
-        <v>177</v>
+      <c r="A47" s="45" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="39" t="s">
-        <v>178</v>
+      <c r="A48" s="44" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="40" t="s">
-        <v>179</v>
+      <c r="A49" s="45" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="40" t="s">
-        <v>180</v>
+      <c r="A50" s="45" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="40" t="s">
-        <v>181</v>
+      <c r="A51" s="45" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4053,1734 +4206,1734 @@
   </sheetPr>
   <dimension ref="A1:B342"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="41" width="56.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="41" width="45.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="41" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="56.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="46" width="45.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="46" width="11"/>
   </cols>
   <sheetData>
-    <row r="1" s="42" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>182</v>
+    <row r="1" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="41" t="s">
-        <v>183</v>
+      <c r="A2" s="46" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="41" t="s">
-        <v>184</v>
+      <c r="A3" s="46" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="41" t="s">
-        <v>185</v>
+      <c r="A4" s="46" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="41" t="s">
-        <v>186</v>
+      <c r="A5" s="46" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="41" t="s">
-        <v>187</v>
+      <c r="A6" s="46" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="41" t="s">
-        <v>188</v>
+      <c r="A7" s="46" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="41" t="s">
-        <v>189</v>
+      <c r="A8" s="46" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="41" t="s">
-        <v>190</v>
+      <c r="A9" s="46" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="41" t="s">
-        <v>191</v>
+      <c r="A10" s="46" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="41" t="s">
-        <v>192</v>
+      <c r="A11" s="46" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="41" t="s">
-        <v>193</v>
+      <c r="A12" s="46" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="41" t="s">
-        <v>194</v>
+      <c r="A13" s="46" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="41" t="s">
-        <v>195</v>
+      <c r="A14" s="46" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="41" t="s">
-        <v>196</v>
+      <c r="A15" s="46" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="41" t="s">
-        <v>197</v>
+      <c r="A16" s="46" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="41" t="s">
-        <v>198</v>
+      <c r="A17" s="46" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="41" t="s">
-        <v>199</v>
+      <c r="A18" s="46" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="41" t="s">
-        <v>200</v>
+      <c r="A19" s="46" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="41" t="s">
-        <v>201</v>
+      <c r="A20" s="46" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="41" t="s">
-        <v>202</v>
+      <c r="A21" s="46" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="41" t="s">
-        <v>203</v>
+      <c r="A22" s="46" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="41" t="s">
-        <v>204</v>
+      <c r="A23" s="46" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="41" t="s">
-        <v>205</v>
+      <c r="A24" s="46" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="41" t="s">
-        <v>206</v>
+      <c r="A25" s="46" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="41" t="s">
-        <v>207</v>
+      <c r="A26" s="46" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="41" t="s">
-        <v>208</v>
+      <c r="A27" s="46" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="41" t="s">
-        <v>209</v>
+      <c r="A28" s="46" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="41" t="s">
-        <v>210</v>
+      <c r="A29" s="46" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="41" t="s">
-        <v>211</v>
+      <c r="A30" s="46" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="41" t="s">
-        <v>212</v>
+      <c r="A31" s="46" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="41" t="s">
-        <v>213</v>
+      <c r="A32" s="46" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="41" t="s">
-        <v>214</v>
+      <c r="A33" s="46" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="41" t="s">
-        <v>215</v>
+      <c r="A34" s="46" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="41" t="s">
-        <v>216</v>
+      <c r="A35" s="46" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="41" t="s">
-        <v>217</v>
+      <c r="A36" s="46" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="41" t="s">
-        <v>218</v>
+      <c r="A37" s="46" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="41" t="s">
-        <v>219</v>
+      <c r="A38" s="46" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="41" t="s">
-        <v>220</v>
+      <c r="A39" s="46" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="41" t="s">
-        <v>221</v>
+      <c r="A40" s="46" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="41" t="s">
-        <v>222</v>
+      <c r="A41" s="46" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="41" t="s">
-        <v>223</v>
+      <c r="A42" s="46" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="41" t="s">
-        <v>224</v>
+      <c r="A43" s="46" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="41" t="s">
-        <v>225</v>
+      <c r="A44" s="46" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="41" t="s">
-        <v>226</v>
+      <c r="A45" s="46" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="41" t="s">
-        <v>227</v>
+      <c r="A46" s="46" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="41" t="s">
-        <v>228</v>
+      <c r="A47" s="46" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="41" t="s">
-        <v>229</v>
+      <c r="A48" s="46" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="41" t="s">
-        <v>230</v>
+      <c r="A49" s="46" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="41" t="s">
-        <v>231</v>
+      <c r="A50" s="46" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="41" t="s">
-        <v>232</v>
+      <c r="A51" s="46" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="41" t="s">
-        <v>233</v>
+      <c r="A52" s="46" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="41" t="s">
-        <v>234</v>
+      <c r="A53" s="46" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="41" t="s">
-        <v>235</v>
+      <c r="A54" s="46" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="41" t="s">
-        <v>236</v>
+      <c r="A55" s="46" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="41" t="s">
-        <v>237</v>
+      <c r="A56" s="46" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="41" t="s">
-        <v>238</v>
+      <c r="A57" s="46" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="41" t="s">
-        <v>239</v>
+      <c r="A58" s="46" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="41" t="s">
-        <v>240</v>
+      <c r="A59" s="46" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="41" t="s">
-        <v>241</v>
+      <c r="A60" s="46" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="41" t="s">
-        <v>242</v>
+      <c r="A61" s="46" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="41" t="s">
-        <v>243</v>
+      <c r="A62" s="46" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="41" t="s">
-        <v>244</v>
+      <c r="A63" s="46" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="41" t="s">
-        <v>245</v>
+      <c r="A64" s="46" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="41" t="s">
-        <v>246</v>
+      <c r="A65" s="46" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="41" t="s">
-        <v>247</v>
+      <c r="A66" s="46" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="41" t="s">
-        <v>248</v>
+      <c r="A67" s="46" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="41" t="s">
-        <v>249</v>
+      <c r="A68" s="46" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="41" t="s">
-        <v>250</v>
+      <c r="A69" s="46" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="41" t="s">
-        <v>251</v>
+      <c r="A70" s="46" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="41" t="s">
-        <v>252</v>
+      <c r="A71" s="46" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="41" t="s">
-        <v>253</v>
+      <c r="A72" s="46" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="41" t="s">
-        <v>254</v>
+      <c r="A73" s="46" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="41" t="s">
-        <v>255</v>
+      <c r="A74" s="46" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="41" t="s">
-        <v>256</v>
+      <c r="A75" s="46" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="41" t="s">
-        <v>257</v>
+      <c r="A76" s="46" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="41" t="s">
-        <v>258</v>
+      <c r="A77" s="46" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="41" t="s">
-        <v>259</v>
+      <c r="A78" s="46" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="41" t="s">
-        <v>260</v>
+      <c r="A79" s="46" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="41" t="s">
-        <v>261</v>
+      <c r="A80" s="46" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="41" t="s">
-        <v>262</v>
+      <c r="A81" s="46" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="41" t="s">
-        <v>263</v>
+      <c r="A82" s="46" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="41" t="s">
-        <v>264</v>
+      <c r="A83" s="46" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="41" t="s">
-        <v>265</v>
+      <c r="A84" s="46" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="41" t="s">
-        <v>266</v>
+      <c r="A85" s="46" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="41" t="s">
-        <v>267</v>
+      <c r="A86" s="46" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="41" t="s">
-        <v>268</v>
+      <c r="A87" s="46" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="41" t="s">
-        <v>269</v>
+      <c r="A88" s="46" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="41" t="s">
-        <v>270</v>
+      <c r="A89" s="46" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="41" t="s">
-        <v>271</v>
+      <c r="A90" s="46" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="41" t="s">
-        <v>272</v>
+      <c r="A91" s="46" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="41" t="s">
-        <v>273</v>
+      <c r="A92" s="46" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="41" t="s">
-        <v>274</v>
+      <c r="A93" s="46" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="41" t="s">
-        <v>275</v>
+      <c r="A94" s="46" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="41" t="s">
-        <v>276</v>
+      <c r="A95" s="46" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="41" t="s">
-        <v>277</v>
+      <c r="A96" s="46" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="41" t="s">
-        <v>278</v>
+      <c r="A97" s="46" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="41" t="s">
-        <v>279</v>
+      <c r="A98" s="46" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="41" t="s">
-        <v>280</v>
+      <c r="A99" s="46" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="41" t="s">
-        <v>281</v>
+      <c r="A100" s="46" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="41" t="s">
-        <v>282</v>
+      <c r="A101" s="46" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="41" t="s">
-        <v>283</v>
+      <c r="A102" s="46" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="41" t="s">
-        <v>284</v>
+      <c r="A103" s="46" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="41" t="s">
-        <v>285</v>
+      <c r="A104" s="46" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="41" t="s">
-        <v>286</v>
+      <c r="A105" s="46" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="41" t="s">
-        <v>287</v>
+      <c r="A106" s="46" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="41" t="s">
-        <v>288</v>
+      <c r="A107" s="46" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="41" t="s">
-        <v>289</v>
+      <c r="A108" s="46" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="41" t="s">
-        <v>290</v>
+      <c r="A109" s="46" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="41" t="s">
-        <v>291</v>
+      <c r="A110" s="46" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="41" t="s">
-        <v>292</v>
+      <c r="A111" s="46" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="41" t="s">
-        <v>293</v>
+      <c r="A112" s="46" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="41" t="s">
-        <v>294</v>
+      <c r="A113" s="46" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="41" t="s">
-        <v>295</v>
+      <c r="A114" s="46" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="41" t="s">
-        <v>296</v>
+      <c r="A115" s="46" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="41" t="s">
-        <v>297</v>
+      <c r="A116" s="46" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="41" t="s">
-        <v>298</v>
+      <c r="A117" s="46" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="41" t="s">
-        <v>299</v>
+      <c r="A118" s="46" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="41" t="s">
-        <v>300</v>
+      <c r="A119" s="46" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="41" t="s">
-        <v>301</v>
+      <c r="A120" s="46" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="41" t="s">
-        <v>302</v>
+      <c r="A121" s="46" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="41" t="s">
-        <v>303</v>
+      <c r="A122" s="46" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="41" t="s">
-        <v>304</v>
+      <c r="A123" s="46" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="41" t="s">
-        <v>305</v>
+      <c r="A124" s="46" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="41" t="s">
-        <v>306</v>
+      <c r="A125" s="46" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="41" t="s">
-        <v>307</v>
+      <c r="A126" s="46" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="41" t="s">
-        <v>308</v>
+      <c r="A127" s="46" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="41" t="s">
-        <v>309</v>
+      <c r="A128" s="46" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="41" t="s">
-        <v>310</v>
+      <c r="A129" s="46" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="41" t="s">
-        <v>311</v>
+      <c r="A130" s="46" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="41" t="s">
-        <v>312</v>
+      <c r="A131" s="46" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="41" t="s">
-        <v>313</v>
+      <c r="A132" s="46" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="41" t="s">
-        <v>314</v>
+      <c r="A133" s="46" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="41" t="s">
-        <v>315</v>
+      <c r="A134" s="46" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="41" t="s">
-        <v>316</v>
+      <c r="A135" s="46" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="41" t="s">
-        <v>317</v>
+      <c r="A136" s="46" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="41" t="s">
-        <v>318</v>
+      <c r="A137" s="46" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="41" t="s">
-        <v>319</v>
+      <c r="A138" s="46" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="41" t="s">
-        <v>320</v>
+      <c r="A139" s="46" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="41" t="s">
-        <v>321</v>
+      <c r="A140" s="46" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="41" t="s">
-        <v>322</v>
+      <c r="A141" s="46" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="41" t="s">
-        <v>323</v>
+      <c r="A142" s="46" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="41" t="s">
-        <v>324</v>
+      <c r="A143" s="46" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="41" t="s">
-        <v>325</v>
+      <c r="A144" s="46" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="41" t="s">
-        <v>326</v>
+      <c r="A145" s="46" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="41" t="s">
-        <v>327</v>
+      <c r="A146" s="46" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="41" t="s">
-        <v>328</v>
+      <c r="A147" s="46" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="41" t="s">
-        <v>329</v>
+      <c r="A148" s="46" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="41" t="s">
-        <v>330</v>
+      <c r="A149" s="46" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="41" t="s">
-        <v>331</v>
+      <c r="A150" s="46" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="41" t="s">
-        <v>332</v>
+      <c r="A151" s="46" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="41" t="s">
-        <v>333</v>
+      <c r="A152" s="46" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="41" t="s">
-        <v>334</v>
+      <c r="A153" s="46" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="41" t="s">
-        <v>335</v>
+      <c r="A154" s="46" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="41" t="s">
-        <v>336</v>
+      <c r="A155" s="46" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="41" t="s">
-        <v>337</v>
+      <c r="A156" s="46" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="41" t="s">
-        <v>338</v>
+      <c r="A157" s="46" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="41" t="s">
-        <v>339</v>
+      <c r="A158" s="46" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="41" t="s">
-        <v>340</v>
+      <c r="A159" s="46" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="41" t="s">
-        <v>341</v>
+      <c r="A160" s="46" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="41" t="s">
-        <v>342</v>
+      <c r="A161" s="46" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="41" t="s">
-        <v>343</v>
+      <c r="A162" s="46" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="41" t="s">
-        <v>344</v>
+      <c r="A163" s="46" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="41" t="s">
-        <v>345</v>
+      <c r="A164" s="46" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="41" t="s">
-        <v>346</v>
+      <c r="A165" s="46" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="41" t="s">
-        <v>347</v>
+      <c r="A166" s="46" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="41" t="s">
-        <v>348</v>
+      <c r="A167" s="46" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="41" t="s">
-        <v>349</v>
+      <c r="A168" s="46" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="41" t="s">
-        <v>350</v>
+      <c r="A169" s="46" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="41" t="s">
-        <v>351</v>
+      <c r="A170" s="46" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="41" t="s">
-        <v>352</v>
+      <c r="A171" s="46" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="41" t="s">
-        <v>353</v>
+      <c r="A172" s="46" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="41" t="s">
-        <v>354</v>
+      <c r="A173" s="46" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="41" t="s">
-        <v>355</v>
+      <c r="A174" s="46" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="41" t="s">
-        <v>356</v>
+      <c r="A175" s="46" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="41" t="s">
-        <v>357</v>
+      <c r="A176" s="46" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="41" t="s">
-        <v>358</v>
+      <c r="A177" s="46" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="41" t="s">
-        <v>359</v>
+      <c r="A178" s="46" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="41" t="s">
-        <v>360</v>
+      <c r="A179" s="46" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="41" t="s">
-        <v>361</v>
+      <c r="A180" s="46" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="41" t="s">
-        <v>362</v>
+      <c r="A181" s="46" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="41" t="s">
-        <v>363</v>
+      <c r="A182" s="46" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="41" t="s">
-        <v>364</v>
+      <c r="A183" s="46" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="41" t="s">
-        <v>365</v>
+      <c r="A184" s="46" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="41" t="s">
-        <v>366</v>
+      <c r="A185" s="46" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="41" t="s">
-        <v>367</v>
+      <c r="A186" s="46" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="41" t="s">
-        <v>368</v>
+      <c r="A187" s="46" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="41" t="s">
-        <v>369</v>
+      <c r="A188" s="46" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="41" t="s">
-        <v>370</v>
+      <c r="A189" s="46" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="41" t="s">
-        <v>371</v>
+      <c r="A190" s="46" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="41" t="s">
-        <v>372</v>
+      <c r="A191" s="46" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="41" t="s">
-        <v>373</v>
+      <c r="A192" s="46" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="41" t="s">
-        <v>374</v>
+      <c r="A193" s="46" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="41" t="s">
-        <v>375</v>
+      <c r="A194" s="46" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="41" t="s">
-        <v>376</v>
+      <c r="A195" s="46" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="41" t="s">
-        <v>377</v>
+      <c r="A196" s="46" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="41" t="s">
-        <v>378</v>
+      <c r="A197" s="46" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="41" t="s">
-        <v>379</v>
+      <c r="A198" s="46" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="41" t="s">
-        <v>380</v>
+      <c r="A199" s="46" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="41" t="s">
-        <v>381</v>
+      <c r="A200" s="46" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="41" t="s">
-        <v>382</v>
+      <c r="A201" s="46" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="41" t="s">
-        <v>383</v>
+      <c r="A202" s="46" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="41" t="s">
-        <v>384</v>
+      <c r="A203" s="46" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="41" t="s">
-        <v>385</v>
+      <c r="A204" s="46" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="41" t="s">
-        <v>386</v>
+      <c r="A205" s="46" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="41" t="s">
-        <v>387</v>
+      <c r="A206" s="46" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="41" t="s">
-        <v>388</v>
+      <c r="A207" s="46" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="41" t="s">
-        <v>389</v>
+      <c r="A208" s="46" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="41" t="s">
-        <v>390</v>
+      <c r="A209" s="46" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="41" t="s">
-        <v>391</v>
+      <c r="A210" s="46" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="41" t="s">
-        <v>392</v>
+      <c r="A211" s="46" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="41" t="s">
-        <v>393</v>
+      <c r="A212" s="46" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="41" t="s">
-        <v>394</v>
+      <c r="A213" s="46" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="41" t="s">
-        <v>395</v>
+      <c r="A214" s="46" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="41" t="s">
-        <v>396</v>
+      <c r="A215" s="46" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="41" t="s">
-        <v>397</v>
+      <c r="A216" s="46" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="41" t="s">
-        <v>398</v>
+      <c r="A217" s="46" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="41" t="s">
-        <v>399</v>
+      <c r="A218" s="46" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="41" t="s">
-        <v>400</v>
+      <c r="A219" s="46" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="41" t="s">
-        <v>401</v>
+      <c r="A220" s="46" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="41" t="s">
-        <v>402</v>
+      <c r="A221" s="46" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="41" t="s">
-        <v>403</v>
+      <c r="A222" s="46" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="41" t="s">
-        <v>404</v>
+      <c r="A223" s="46" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="41" t="s">
-        <v>405</v>
+      <c r="A224" s="46" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="41" t="s">
-        <v>406</v>
+      <c r="A225" s="46" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="41" t="s">
-        <v>407</v>
+      <c r="A226" s="46" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="41" t="s">
-        <v>408</v>
+      <c r="A227" s="46" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="41" t="s">
-        <v>409</v>
+      <c r="A228" s="46" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="41" t="s">
-        <v>410</v>
+      <c r="A229" s="46" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="41" t="s">
-        <v>411</v>
+      <c r="A230" s="46" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="41" t="s">
-        <v>412</v>
+      <c r="A231" s="46" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="41" t="s">
-        <v>413</v>
+      <c r="A232" s="46" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="41" t="s">
-        <v>414</v>
+      <c r="A233" s="46" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="41" t="s">
-        <v>415</v>
+      <c r="A234" s="46" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="41" t="s">
-        <v>416</v>
+      <c r="A235" s="46" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="41" t="s">
-        <v>417</v>
+      <c r="A236" s="46" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="41" t="s">
-        <v>418</v>
+      <c r="A237" s="46" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="41" t="s">
-        <v>419</v>
+      <c r="A238" s="46" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="41" t="s">
-        <v>420</v>
+      <c r="A239" s="46" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="41" t="s">
-        <v>421</v>
+      <c r="A240" s="46" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="41" t="s">
-        <v>422</v>
+      <c r="A241" s="46" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="41" t="s">
-        <v>423</v>
+      <c r="A242" s="46" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="41" t="s">
-        <v>424</v>
+      <c r="A243" s="46" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="41" t="s">
-        <v>425</v>
+      <c r="A244" s="46" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="41" t="s">
-        <v>426</v>
+      <c r="A245" s="46" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="41" t="s">
-        <v>427</v>
+      <c r="A246" s="46" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="41" t="s">
-        <v>428</v>
+      <c r="A247" s="46" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="41" t="s">
-        <v>429</v>
+      <c r="A248" s="46" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="41" t="s">
-        <v>430</v>
+      <c r="A249" s="46" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="41" t="s">
-        <v>431</v>
+      <c r="A250" s="46" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="41" t="s">
-        <v>432</v>
+      <c r="A251" s="46" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="41" t="s">
-        <v>433</v>
+      <c r="A252" s="46" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="41" t="s">
-        <v>434</v>
+      <c r="A253" s="46" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="41" t="s">
-        <v>435</v>
+      <c r="A254" s="46" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="41" t="s">
-        <v>436</v>
+      <c r="A255" s="46" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="41" t="s">
-        <v>437</v>
+      <c r="A256" s="46" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="41" t="s">
-        <v>438</v>
+      <c r="A257" s="46" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="41" t="s">
-        <v>439</v>
+      <c r="A258" s="46" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="41" t="s">
-        <v>440</v>
+      <c r="A259" s="46" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="41" t="s">
-        <v>441</v>
+      <c r="A260" s="46" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="41" t="s">
-        <v>442</v>
+      <c r="A261" s="46" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="41" t="s">
-        <v>443</v>
+      <c r="A262" s="46" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="41" t="s">
-        <v>444</v>
+      <c r="A263" s="46" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="41" t="s">
-        <v>445</v>
+      <c r="A264" s="46" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="41" t="s">
-        <v>446</v>
+      <c r="A265" s="46" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="41" t="s">
-        <v>447</v>
+      <c r="A266" s="46" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="41" t="s">
-        <v>448</v>
+      <c r="A267" s="46" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="41" t="s">
-        <v>449</v>
+      <c r="A268" s="46" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="41" t="s">
-        <v>450</v>
+      <c r="A269" s="46" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="41" t="s">
-        <v>451</v>
+      <c r="A270" s="46" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="41" t="s">
-        <v>452</v>
+      <c r="A271" s="46" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="41" t="s">
-        <v>453</v>
+      <c r="A272" s="46" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="41" t="s">
-        <v>454</v>
+      <c r="A273" s="46" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="41" t="s">
-        <v>455</v>
+      <c r="A274" s="46" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="41" t="s">
-        <v>456</v>
+      <c r="A275" s="46" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="41" t="s">
-        <v>457</v>
+      <c r="A276" s="46" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="41" t="s">
-        <v>458</v>
+      <c r="A277" s="46" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="41" t="s">
-        <v>459</v>
+      <c r="A278" s="46" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="41" t="s">
-        <v>460</v>
+      <c r="A279" s="46" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="41" t="s">
-        <v>461</v>
+      <c r="A280" s="46" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="41" t="s">
-        <v>462</v>
+      <c r="A281" s="46" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="41" t="s">
-        <v>463</v>
+      <c r="A282" s="46" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="41" t="s">
-        <v>464</v>
+      <c r="A283" s="46" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="41" t="s">
-        <v>465</v>
+      <c r="A284" s="46" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="41" t="s">
-        <v>466</v>
+      <c r="A285" s="46" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="41" t="s">
-        <v>467</v>
+      <c r="A286" s="46" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="41" t="s">
-        <v>468</v>
+      <c r="A287" s="46" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="41" t="s">
-        <v>469</v>
+      <c r="A288" s="46" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="41" t="s">
-        <v>470</v>
+      <c r="A289" s="46" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="41" t="s">
-        <v>471</v>
+      <c r="A290" s="46" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="41" t="s">
-        <v>472</v>
+      <c r="A291" s="46" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="41" t="s">
-        <v>473</v>
+      <c r="A292" s="46" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="41" t="s">
-        <v>474</v>
+      <c r="A293" s="46" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="41" t="s">
-        <v>475</v>
+      <c r="A294" s="46" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A295" s="41" t="s">
-        <v>476</v>
+      <c r="A295" s="46" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="41" t="s">
-        <v>477</v>
+      <c r="A296" s="46" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="41" t="s">
-        <v>478</v>
+      <c r="A297" s="46" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A298" s="41" t="s">
-        <v>479</v>
+      <c r="A298" s="46" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="41" t="s">
-        <v>480</v>
+      <c r="A299" s="46" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A300" s="41" t="s">
-        <v>481</v>
+      <c r="A300" s="46" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A301" s="41" t="s">
-        <v>482</v>
+      <c r="A301" s="46" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="41" t="s">
-        <v>483</v>
+      <c r="A302" s="46" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A303" s="41" t="s">
-        <v>484</v>
+      <c r="A303" s="46" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="41" t="s">
-        <v>485</v>
+      <c r="A304" s="46" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A305" s="41" t="s">
-        <v>486</v>
+      <c r="A305" s="46" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A306" s="41" t="s">
-        <v>487</v>
+      <c r="A306" s="46" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A307" s="41" t="s">
-        <v>488</v>
+      <c r="A307" s="46" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A308" s="41" t="s">
-        <v>489</v>
+      <c r="A308" s="46" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A309" s="41" t="s">
-        <v>490</v>
+      <c r="A309" s="46" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A310" s="41" t="s">
-        <v>491</v>
+      <c r="A310" s="46" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A311" s="41" t="s">
-        <v>492</v>
+      <c r="A311" s="46" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A312" s="41" t="s">
-        <v>493</v>
+      <c r="A312" s="46" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A313" s="41" t="s">
-        <v>494</v>
+      <c r="A313" s="46" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A314" s="41" t="s">
-        <v>495</v>
+      <c r="A314" s="46" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A315" s="41" t="s">
-        <v>496</v>
+      <c r="A315" s="46" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A316" s="41" t="s">
-        <v>497</v>
+      <c r="A316" s="46" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A317" s="41" t="s">
-        <v>498</v>
+      <c r="A317" s="46" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A318" s="41" t="s">
-        <v>499</v>
+      <c r="A318" s="46" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A319" s="41" t="s">
-        <v>500</v>
+      <c r="A319" s="46" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A320" s="41" t="s">
-        <v>501</v>
+      <c r="A320" s="46" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A321" s="41" t="s">
-        <v>502</v>
+      <c r="A321" s="46" t="s">
+        <v>509</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A322" s="41" t="s">
-        <v>503</v>
+      <c r="A322" s="46" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A323" s="41" t="s">
-        <v>504</v>
+      <c r="A323" s="46" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A324" s="41" t="s">
-        <v>505</v>
+      <c r="A324" s="46" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A325" s="41" t="s">
-        <v>506</v>
+      <c r="A325" s="46" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A326" s="41" t="s">
-        <v>507</v>
+      <c r="A326" s="46" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A327" s="41" t="s">
-        <v>508</v>
+      <c r="A327" s="46" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A328" s="41" t="s">
-        <v>509</v>
+      <c r="A328" s="46" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A329" s="41" t="s">
-        <v>510</v>
+      <c r="A329" s="46" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A330" s="41" t="s">
-        <v>511</v>
+      <c r="A330" s="46" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A331" s="41" t="s">
-        <v>512</v>
+      <c r="A331" s="46" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A332" s="41" t="s">
-        <v>513</v>
+      <c r="A332" s="46" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A333" s="41" t="s">
-        <v>514</v>
+      <c r="A333" s="46" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A334" s="41" t="s">
-        <v>515</v>
+      <c r="A334" s="46" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A335" s="41" t="s">
-        <v>516</v>
+      <c r="A335" s="46" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A336" s="41" t="s">
-        <v>517</v>
+      <c r="A336" s="46" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A337" s="41" t="s">
-        <v>518</v>
+      <c r="A337" s="46" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A338" s="41" t="s">
-        <v>519</v>
+      <c r="A338" s="46" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A339" s="41" t="s">
-        <v>520</v>
+      <c r="A339" s="46" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A340" s="41" t="s">
-        <v>521</v>
+      <c r="A340" s="46" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A341" s="41" t="s">
-        <v>522</v>
+      <c r="A341" s="46" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A342" s="41" t="s">
-        <v>523</v>
+      <c r="A342" s="46" t="s">
+        <v>530</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5795,165 +5948,165 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="36" width="31.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="36" width="27.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="36" width="25.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="36" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="36" width="27.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="36" width="28"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="36" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="41" width="31.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="41" width="27.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="41" width="25.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="41" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="41" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="41" width="28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="41" width="11"/>
   </cols>
   <sheetData>
-    <row r="1" s="38" customFormat="true" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>524</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>525</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>526</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>527</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>528</v>
+    <row r="1" s="43" customFormat="true" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>531</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>532</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>533</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>534</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="43" t="s">
-        <v>529</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>530</v>
-      </c>
-      <c r="C2" s="43" t="s">
-        <v>530</v>
-      </c>
-      <c r="D2" s="43" t="s">
-        <v>530</v>
-      </c>
-      <c r="E2" s="43" t="s">
-        <v>531</v>
-      </c>
-      <c r="F2" s="43" t="s">
-        <v>532</v>
+      <c r="A2" s="48" t="s">
+        <v>536</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>537</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>537</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>537</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>538</v>
+      </c>
+      <c r="F2" s="48" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="43" t="s">
-        <v>533</v>
-      </c>
-      <c r="B3" s="43" t="s">
-        <v>534</v>
-      </c>
-      <c r="C3" s="43" t="s">
-        <v>534</v>
-      </c>
-      <c r="D3" s="43" t="s">
-        <v>535</v>
-      </c>
-      <c r="E3" s="43" t="s">
-        <v>536</v>
-      </c>
-      <c r="F3" s="43" t="s">
+      <c r="A3" s="48" t="s">
+        <v>540</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>541</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>541</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>542</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>543</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="48" t="s">
+        <v>545</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>541</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>541</v>
+      </c>
+      <c r="D4" s="48" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="43" t="s">
+      <c r="E4" s="48" t="s">
+        <v>543</v>
+      </c>
+      <c r="F4" s="48" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>544</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>544</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>541</v>
+      </c>
+      <c r="E5" s="48" t="s">
         <v>538</v>
       </c>
-      <c r="B4" s="43" t="s">
-        <v>534</v>
-      </c>
-      <c r="C4" s="43" t="s">
-        <v>534</v>
-      </c>
-      <c r="D4" s="43" t="s">
-        <v>530</v>
-      </c>
-      <c r="E4" s="43" t="s">
-        <v>536</v>
-      </c>
-      <c r="F4" s="43" t="s">
+      <c r="F5" s="48" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="48" t="s">
+        <v>547</v>
+      </c>
+      <c r="B6" s="48" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="43" t="s">
+      <c r="C6" s="48" t="s">
+        <v>541</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>537</v>
+      </c>
+      <c r="E6" s="48" t="s">
+        <v>543</v>
+      </c>
+      <c r="F6" s="48" t="s">
         <v>539</v>
       </c>
-      <c r="B5" s="43" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="48" t="s">
+        <v>548</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>544</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>544</v>
+      </c>
+      <c r="D7" s="48" t="s">
         <v>537</v>
       </c>
-      <c r="C5" s="43" t="s">
-        <v>537</v>
-      </c>
-      <c r="D5" s="43" t="s">
-        <v>534</v>
-      </c>
-      <c r="E5" s="43" t="s">
-        <v>531</v>
-      </c>
-      <c r="F5" s="43" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="43" t="s">
-        <v>540</v>
-      </c>
-      <c r="B6" s="43" t="s">
-        <v>530</v>
-      </c>
-      <c r="C6" s="43" t="s">
-        <v>534</v>
-      </c>
-      <c r="D6" s="43" t="s">
-        <v>530</v>
-      </c>
-      <c r="E6" s="43" t="s">
-        <v>536</v>
-      </c>
-      <c r="F6" s="43" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="43" t="s">
-        <v>541</v>
-      </c>
-      <c r="B7" s="43" t="s">
-        <v>537</v>
-      </c>
-      <c r="C7" s="43" t="s">
-        <v>537</v>
-      </c>
-      <c r="D7" s="43" t="s">
-        <v>530</v>
-      </c>
-      <c r="E7" s="43" t="s">
-        <v>536</v>
-      </c>
-      <c r="F7" s="43" t="s">
-        <v>542</v>
+      <c r="E7" s="48" t="s">
+        <v>543</v>
+      </c>
+      <c r="F7" s="48" t="s">
+        <v>549</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>